<commit_message>
Modified code in Test Class- LoginPageTest
</commit_message>
<xml_diff>
--- a/KhanAcademy/src/test/resources/testData/TestData.xlsx
+++ b/KhanAcademy/src/test/resources/testData/TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15255" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15255" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="4" r:id="rId1"/>
+    <sheet name="EditProfileData" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:O18"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>userName</t>
   </si>
@@ -27,13 +28,49 @@
   </si>
   <si>
     <t>ankush18</t>
+  </si>
+  <si>
+    <t>NICKNAME</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>Ankush Nikure</t>
+  </si>
+  <si>
+    <t>I'm having around 3+ years of experience into IT as a QA (Engineer) in Manual &amp; Automation Testing.
+But from last 1year/2year I'm majorly involved in Automation activities.</t>
+  </si>
+  <si>
+    <t>Ankush</t>
+  </si>
+  <si>
+    <t>ankush1234</t>
+  </si>
+  <si>
+    <t>I'm involved Frontend Automation (as well as Backened Automation).
+From Frontend Automation pov, we are using Selenium WebDriver with Java language binding.</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>But my major roles &amp; responsibilities is into Automation, I would say 70-80 % into Automation.
+But we are doing 20-30 % Manual Testing (Functional) as well.</t>
+  </si>
+  <si>
+    <t>123456789!#$%^&amp;*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,6 +82,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -87,16 +132,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -436,4 +515,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>12345678</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9">
+        <v>54654849</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2" display="!@#$%^^&amp;*"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>